<commit_message>
after full access_import 13_10_21; added acces import-setup, scripts and data
</commit_message>
<xml_diff>
--- a/data/EXCEL-ACCESS_Kürzel-Titel-Orden-2021-01-28.xlsx
+++ b/data/EXCEL-ACCESS_Kürzel-Titel-Orden-2021-01-28.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mr/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregorpirgie/gregor/arbeit/acdh/viecpro_import_for_upload/viecpro_import_app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{375A48B5-87FE-414D-AC8E-48E6CA369CC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F71B10A-8149-5B44-87CF-E014C2485C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{5CCB960F-3AFE-C544-B885-C68705E33573}"/>
+    <workbookView xWindow="26560" yWindow="-2040" windowWidth="25600" windowHeight="15500" xr2:uid="{5CCB960F-3AFE-C544-B885-C68705E33573}"/>
   </bookViews>
   <sheets>
     <sheet name="Titel" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="570">
   <si>
     <t>REGEL für EXCEL: Kürzel vereinheitlichen und alle enthaltenen Fragezeichen ? ebenfalls importieren!</t>
   </si>
@@ -1758,12 +1758,18 @@
   <si>
     <t>unter Funktion tun, kann auch manuell gemacht werden, da es selten vorkommt</t>
   </si>
+  <si>
+    <t>Freifrau von</t>
+  </si>
+  <si>
+    <t>Freifrau v.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1988,7 +1994,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2101,6 +2107,18 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2330,13 +2348,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -2377,6 +2388,13 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2415,8 +2433,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FD749BC9-947B-374A-BD0A-6EEAEC63875A}" name="Tabelle612" displayName="Tabelle612" ref="A4:F244" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7">
-  <autoFilter ref="A4:F244" xr:uid="{488391E5-2445-4346-A803-BFDFD62C3CCB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FD749BC9-947B-374A-BD0A-6EEAEC63875A}" name="Tabelle612" displayName="Tabelle612" ref="A4:F245" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+  <autoFilter ref="A4:F245" xr:uid="{488391E5-2445-4346-A803-BFDFD62C3CCB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:F244">
     <sortCondition ref="D4:D244"/>
   </sortState>
@@ -2433,7 +2451,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2731,26 +2749,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAECCBE5-B06E-1A44-BAF8-2274F664AD2C}">
   <dimension ref="A1:F492"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A242" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="B247" sqref="B247"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="22" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="32" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="27" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="32.1">
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
@@ -2762,7 +2780,7 @@
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
     </row>
-    <row r="4" spans="1:6" s="31" customFormat="1" ht="48">
+    <row r="4" spans="1:6" s="31" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
@@ -2782,7 +2800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="36">
+    <row r="5" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -2802,7 +2820,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24">
+    <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2822,7 +2840,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="36">
+    <row r="7" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -2842,7 +2860,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="36">
+    <row r="8" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2862,7 +2880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="36">
+    <row r="9" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2882,7 +2900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="24">
+    <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -2902,7 +2920,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="36">
+    <row r="11" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
@@ -2922,7 +2940,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="36">
+    <row r="12" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>29</v>
       </c>
@@ -2942,7 +2960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="60">
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
@@ -2962,7 +2980,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="24">
+    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>36</v>
       </c>
@@ -2982,7 +3000,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="24">
+    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
@@ -3002,7 +3020,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="24">
+    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>40</v>
       </c>
@@ -3022,7 +3040,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="36">
+    <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>42</v>
       </c>
@@ -3042,7 +3060,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="36">
+    <row r="18" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>44</v>
       </c>
@@ -3062,7 +3080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="24">
+    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -3082,7 +3100,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="24">
+    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>48</v>
       </c>
@@ -3102,7 +3120,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="36">
+    <row r="21" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>52</v>
       </c>
@@ -3122,7 +3140,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="24">
+    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>54</v>
       </c>
@@ -3140,7 +3158,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="36">
+    <row r="23" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>57</v>
       </c>
@@ -3158,7 +3176,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="48">
+    <row r="24" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
         <v>62</v>
       </c>
@@ -3176,7 +3194,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="84">
+    <row r="25" spans="1:6" ht="72" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>65</v>
       </c>
@@ -3194,7 +3212,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60">
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>69</v>
       </c>
@@ -3212,7 +3230,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="48">
+    <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>71</v>
       </c>
@@ -3230,7 +3248,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.95">
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>74</v>
       </c>
@@ -3246,7 +3264,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.95">
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>75</v>
       </c>
@@ -3262,7 +3280,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="24">
+    <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>77</v>
       </c>
@@ -3280,7 +3298,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="36">
+    <row r="31" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>79</v>
       </c>
@@ -3298,7 +3316,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="273">
+    <row r="32" spans="1:6" ht="273" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>81</v>
       </c>
@@ -3316,7 +3334,7 @@
       </c>
       <c r="F32" s="23"/>
     </row>
-    <row r="33" spans="1:6" ht="72">
+    <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>85</v>
       </c>
@@ -3334,7 +3352,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.95">
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>89</v>
       </c>
@@ -3350,7 +3368,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="96">
+    <row r="35" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>90</v>
       </c>
@@ -3370,7 +3388,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="132">
+    <row r="36" spans="1:6" ht="132" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>94</v>
       </c>
@@ -3390,7 +3408,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="36">
+    <row r="37" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>99</v>
       </c>
@@ -3408,7 +3426,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="24">
+    <row r="38" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>103</v>
       </c>
@@ -3426,7 +3444,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="60">
+    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>106</v>
       </c>
@@ -3444,7 +3462,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="36">
+    <row r="40" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>109</v>
       </c>
@@ -3462,7 +3480,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="36">
+    <row r="41" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>112</v>
       </c>
@@ -3480,7 +3498,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="48">
+    <row r="42" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>116</v>
       </c>
@@ -3498,7 +3516,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="84">
+    <row r="43" spans="1:6" ht="84" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>119</v>
       </c>
@@ -3516,7 +3534,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="84">
+    <row r="44" spans="1:6" ht="84" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>122</v>
       </c>
@@ -3534,7 +3552,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="48">
+    <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>123</v>
       </c>
@@ -3552,7 +3570,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="48">
+    <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
         <v>127</v>
       </c>
@@ -3570,7 +3588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="48">
+    <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>130</v>
       </c>
@@ -3588,7 +3606,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="24">
+    <row r="48" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>134</v>
       </c>
@@ -3606,7 +3624,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="36">
+    <row r="49" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>137</v>
       </c>
@@ -3624,7 +3642,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="36">
+    <row r="50" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>140</v>
       </c>
@@ -3642,7 +3660,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="24">
+    <row r="51" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="s">
         <v>144</v>
       </c>
@@ -3660,7 +3678,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="24">
+    <row r="52" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>147</v>
       </c>
@@ -3678,7 +3696,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="48">
+    <row r="53" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>150</v>
       </c>
@@ -3696,7 +3714,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="84">
+    <row r="54" spans="1:6" ht="84" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>153</v>
       </c>
@@ -3716,7 +3734,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="48">
+    <row r="55" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
         <v>158</v>
       </c>
@@ -3734,7 +3752,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="24">
+    <row r="56" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
         <v>162</v>
       </c>
@@ -3752,7 +3770,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="36">
+    <row r="57" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
         <v>164</v>
       </c>
@@ -3770,7 +3788,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="36">
+    <row r="58" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>167</v>
       </c>
@@ -3788,7 +3806,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.95">
+    <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
         <v>171</v>
       </c>
@@ -3804,7 +3822,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="63.95">
+    <row r="60" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
         <v>172</v>
       </c>
@@ -3822,7 +3840,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="48">
+    <row r="61" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
         <v>176</v>
       </c>
@@ -3840,7 +3858,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="60">
+    <row r="62" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
         <v>179</v>
       </c>
@@ -3858,7 +3876,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="32.1">
+    <row r="63" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
         <v>183</v>
       </c>
@@ -3876,7 +3894,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="32.1">
+    <row r="64" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
         <v>185</v>
       </c>
@@ -3894,7 +3912,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="24">
+    <row r="65" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="s">
         <v>188</v>
       </c>
@@ -3912,7 +3930,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="36">
+    <row r="66" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
         <v>191</v>
       </c>
@@ -3930,7 +3948,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="24">
+    <row r="67" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A67" s="12" t="s">
         <v>194</v>
       </c>
@@ -3948,7 +3966,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="24">
+    <row r="68" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
         <v>196</v>
       </c>
@@ -3966,7 +3984,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="24">
+    <row r="69" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
         <v>198</v>
       </c>
@@ -3984,7 +4002,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="36">
+    <row r="70" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
         <v>200</v>
       </c>
@@ -4002,7 +4020,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="24">
+    <row r="71" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A71" s="9" t="s">
         <v>202</v>
       </c>
@@ -4020,7 +4038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="48">
+    <row r="72" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
         <v>204</v>
       </c>
@@ -4038,7 +4056,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="48">
+    <row r="73" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
         <v>208</v>
       </c>
@@ -4056,7 +4074,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="60">
+    <row r="74" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
         <v>210</v>
       </c>
@@ -4076,7 +4094,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="36">
+    <row r="75" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
         <v>214</v>
       </c>
@@ -4096,7 +4114,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.95">
+    <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="12" t="s">
         <v>219</v>
       </c>
@@ -4114,7 +4132,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="60">
+    <row r="77" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A77" s="14" t="s">
         <v>222</v>
       </c>
@@ -4132,7 +4150,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="32.1">
+    <row r="78" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
         <v>225</v>
       </c>
@@ -4146,7 +4164,7 @@
       <c r="E78" s="23"/>
       <c r="F78" s="23"/>
     </row>
-    <row r="79" spans="1:6" ht="168">
+    <row r="79" spans="1:6" ht="168" x14ac:dyDescent="0.2">
       <c r="A79" s="14" t="s">
         <v>227</v>
       </c>
@@ -4166,7 +4184,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="72">
+    <row r="80" spans="1:6" ht="72" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>231</v>
       </c>
@@ -4186,7 +4204,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.95">
+    <row r="81" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>236</v>
       </c>
@@ -4204,7 +4222,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.95">
+    <row r="82" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
         <v>239</v>
       </c>
@@ -4222,7 +4240,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="48">
+    <row r="83" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>241</v>
       </c>
@@ -4242,7 +4260,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="24">
+    <row r="84" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>244</v>
       </c>
@@ -4262,7 +4280,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.95">
+    <row r="85" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>248</v>
       </c>
@@ -4280,7 +4298,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.95">
+    <row r="86" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>251</v>
       </c>
@@ -4298,7 +4316,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.95">
+    <row r="87" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
         <v>254</v>
       </c>
@@ -4316,7 +4334,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="24">
+    <row r="88" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>258</v>
       </c>
@@ -4334,7 +4352,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.95">
+    <row r="89" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>261</v>
       </c>
@@ -4352,7 +4370,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15.95">
+    <row r="90" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
         <v>263</v>
       </c>
@@ -4370,7 +4388,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15.95">
+    <row r="91" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
         <v>265</v>
       </c>
@@ -4388,7 +4406,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15.95">
+    <row r="92" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
         <v>266</v>
       </c>
@@ -4408,7 +4426,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15.95">
+    <row r="93" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
         <v>270</v>
       </c>
@@ -4426,7 +4444,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15.95">
+    <row r="94" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
         <v>272</v>
       </c>
@@ -4444,7 +4462,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15.95">
+    <row r="95" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
         <v>273</v>
       </c>
@@ -4462,7 +4480,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15.95">
+    <row r="96" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
         <v>274</v>
       </c>
@@ -4480,7 +4498,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15.95">
+    <row r="97" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
         <v>276</v>
       </c>
@@ -4498,7 +4516,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="36">
+    <row r="98" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A98" s="8" t="s">
         <v>277</v>
       </c>
@@ -4516,7 +4534,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="24">
+    <row r="99" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A99" s="8" t="s">
         <v>279</v>
       </c>
@@ -4534,7 +4552,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="24">
+    <row r="100" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
         <v>282</v>
       </c>
@@ -4554,7 +4572,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15.95">
+    <row r="101" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>286</v>
       </c>
@@ -4572,7 +4590,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15.95">
+    <row r="102" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>288</v>
       </c>
@@ -4590,7 +4608,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="60">
+    <row r="103" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>289</v>
       </c>
@@ -4610,7 +4628,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="72">
+    <row r="104" spans="1:6" ht="72" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>293</v>
       </c>
@@ -4630,7 +4648,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="24">
+    <row r="105" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>297</v>
       </c>
@@ -4650,7 +4668,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="60">
+    <row r="106" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
         <v>301</v>
       </c>
@@ -4670,7 +4688,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="15.95">
+    <row r="107" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>305</v>
       </c>
@@ -4688,7 +4706,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15.95">
+    <row r="108" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>307</v>
       </c>
@@ -4706,7 +4724,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15.95">
+    <row r="109" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>309</v>
       </c>
@@ -4724,7 +4742,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15.95">
+    <row r="110" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="s">
         <v>311</v>
       </c>
@@ -4742,7 +4760,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="15.95">
+    <row r="111" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
         <v>312</v>
       </c>
@@ -4760,7 +4778,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="48">
+    <row r="112" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
         <v>313</v>
       </c>
@@ -4780,7 +4798,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="15.95">
+    <row r="113" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
         <v>318</v>
       </c>
@@ -4798,7 +4816,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="24">
+    <row r="114" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="s">
         <v>320</v>
       </c>
@@ -4816,7 +4834,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15.95">
+    <row r="115" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
         <v>322</v>
       </c>
@@ -4834,7 +4852,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="48">
+    <row r="116" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
         <v>323</v>
       </c>
@@ -4854,7 +4872,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="60">
+    <row r="117" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
         <v>326</v>
       </c>
@@ -4874,7 +4892,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15.95">
+    <row r="118" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="8" t="s">
         <v>330</v>
       </c>
@@ -4892,7 +4910,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15.95">
+    <row r="119" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="8" t="s">
         <v>331</v>
       </c>
@@ -4910,7 +4928,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="24">
+    <row r="120" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A120" s="6" t="s">
         <v>332</v>
       </c>
@@ -4930,7 +4948,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="24">
+    <row r="121" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>337</v>
       </c>
@@ -4950,7 +4968,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="24">
+    <row r="122" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
         <v>340</v>
       </c>
@@ -4970,7 +4988,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="15.95">
+    <row r="123" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>343</v>
       </c>
@@ -4988,7 +5006,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="24">
+    <row r="124" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>344</v>
       </c>
@@ -5006,7 +5024,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="32.1">
+    <row r="125" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>346</v>
       </c>
@@ -5024,7 +5042,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="60">
+    <row r="126" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A126" s="6" t="s">
         <v>349</v>
       </c>
@@ -5042,7 +5060,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="24">
+    <row r="127" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A127" s="8" t="s">
         <v>351</v>
       </c>
@@ -5060,7 +5078,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="24">
+    <row r="128" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
         <v>352</v>
       </c>
@@ -5078,7 +5096,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="15.95">
+    <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>355</v>
       </c>
@@ -5096,7 +5114,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="24">
+    <row r="130" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A130" s="8" t="s">
         <v>356</v>
       </c>
@@ -5114,7 +5132,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="24">
+    <row r="131" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A131" s="6" t="s">
         <v>357</v>
       </c>
@@ -5134,7 +5152,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="24">
+    <row r="132" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A132" s="8" t="s">
         <v>361</v>
       </c>
@@ -5152,7 +5170,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="24">
+    <row r="133" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A133" s="5" t="s">
         <v>363</v>
       </c>
@@ -5170,7 +5188,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="24">
+    <row r="134" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A134" s="8" t="s">
         <v>366</v>
       </c>
@@ -5188,7 +5206,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="24">
+    <row r="135" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
         <v>367</v>
       </c>
@@ -5206,7 +5224,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="15.95">
+    <row r="136" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="6" t="s">
         <v>370</v>
       </c>
@@ -5226,7 +5244,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="24">
+    <row r="137" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A137" s="8" t="s">
         <v>374</v>
       </c>
@@ -5244,7 +5262,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="15.95">
+    <row r="138" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
         <v>375</v>
       </c>
@@ -5262,7 +5280,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="15.95">
+    <row r="139" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="8" t="s">
         <v>376</v>
       </c>
@@ -5280,7 +5298,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="15.95">
+    <row r="140" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="6" t="s">
         <v>378</v>
       </c>
@@ -5298,7 +5316,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="24">
+    <row r="141" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A141" s="6" t="s">
         <v>380</v>
       </c>
@@ -5318,7 +5336,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="24">
+    <row r="142" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A142" s="8" t="s">
         <v>383</v>
       </c>
@@ -5338,7 +5356,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="15.95">
+    <row r="143" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>386</v>
       </c>
@@ -5356,7 +5374,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="24">
+    <row r="144" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
         <v>388</v>
       </c>
@@ -5376,7 +5394,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="15.95">
+    <row r="145" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
         <v>392</v>
       </c>
@@ -5394,7 +5412,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="48">
+    <row r="146" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A146" s="5" t="s">
         <v>393</v>
       </c>
@@ -5414,7 +5432,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="84">
+    <row r="147" spans="1:6" ht="84" x14ac:dyDescent="0.2">
       <c r="A147" s="7" t="s">
         <v>397</v>
       </c>
@@ -5434,7 +5452,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="27.95" customHeight="1">
+    <row r="148" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="8" t="s">
         <v>401</v>
       </c>
@@ -5452,7 +5470,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="15.95">
+    <row r="149" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="8" t="s">
         <v>404</v>
       </c>
@@ -5470,7 +5488,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="24">
+    <row r="150" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
         <v>405</v>
       </c>
@@ -5490,7 +5508,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="36">
+    <row r="151" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
         <v>408</v>
       </c>
@@ -5510,7 +5528,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="15.95">
+    <row r="152" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="7" t="s">
         <v>411</v>
       </c>
@@ -5530,7 +5548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="15.95">
+    <row r="153" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="s">
         <v>413</v>
       </c>
@@ -5550,7 +5568,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="15.95">
+    <row r="154" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
         <v>415</v>
       </c>
@@ -5570,7 +5588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="24">
+    <row r="155" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="s">
         <v>418</v>
       </c>
@@ -5590,7 +5608,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="24">
+    <row r="156" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
         <v>421</v>
       </c>
@@ -5610,7 +5628,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="15.95">
+    <row r="157" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="7" t="s">
         <v>424</v>
       </c>
@@ -5630,7 +5648,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="24">
+    <row r="158" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A158" s="6" t="s">
         <v>426</v>
       </c>
@@ -5650,7 +5668,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="36">
+    <row r="159" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A159" s="6" t="s">
         <v>430</v>
       </c>
@@ -5668,7 +5686,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="24">
+    <row r="160" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A160" s="7" t="s">
         <v>432</v>
       </c>
@@ -5688,7 +5706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="15.95">
+    <row r="161" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
         <v>434</v>
       </c>
@@ -5706,7 +5724,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="15.95">
+    <row r="162" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="8" t="s">
         <v>435</v>
       </c>
@@ -5724,7 +5742,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="15.95">
+    <row r="163" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
         <v>436</v>
       </c>
@@ -5742,7 +5760,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="36">
+    <row r="164" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
         <v>437</v>
       </c>
@@ -5760,7 +5778,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="15.95">
+    <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="8" t="s">
         <v>440</v>
       </c>
@@ -5778,7 +5796,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="24">
+    <row r="166" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A166" s="8" t="s">
         <v>441</v>
       </c>
@@ -5796,7 +5814,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="24">
+    <row r="167" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A167" s="8" t="s">
         <v>442</v>
       </c>
@@ -5814,7 +5832,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="15.95">
+    <row r="168" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="6" t="s">
         <v>443</v>
       </c>
@@ -5832,7 +5850,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="15.95">
+    <row r="169" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="8" t="s">
         <v>444</v>
       </c>
@@ -5850,7 +5868,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="15.95">
+    <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="6" t="s">
         <v>445</v>
       </c>
@@ -5868,7 +5886,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="15.95">
+    <row r="171" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="8" t="s">
         <v>446</v>
       </c>
@@ -5886,7 +5904,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="24">
+    <row r="172" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A172" s="8" t="s">
         <v>447</v>
       </c>
@@ -5904,7 +5922,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="15.95">
+    <row r="173" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="6" t="s">
         <v>449</v>
       </c>
@@ -5922,7 +5940,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="24">
+    <row r="174" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A174" s="8" t="s">
         <v>450</v>
       </c>
@@ -5940,7 +5958,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="15.95">
+    <row r="175" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="6" t="s">
         <v>451</v>
       </c>
@@ -5958,7 +5976,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="15.95">
+    <row r="176" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="8" t="s">
         <v>452</v>
       </c>
@@ -5976,7 +5994,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="15.95">
+    <row r="177" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="8" t="s">
         <v>453</v>
       </c>
@@ -5994,7 +6012,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="15.95">
+    <row r="178" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="8" t="s">
         <v>454</v>
       </c>
@@ -6012,7 +6030,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="15.95">
+    <row r="179" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="7" t="s">
         <v>455</v>
       </c>
@@ -6032,7 +6050,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="15.95">
+    <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="8" t="s">
         <v>456</v>
       </c>
@@ -6050,7 +6068,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="15.95">
+    <row r="181" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A181" s="5" t="s">
         <v>457</v>
       </c>
@@ -6068,7 +6086,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="15.95">
+    <row r="182" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="8" t="s">
         <v>458</v>
       </c>
@@ -6086,7 +6104,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="15.95">
+    <row r="183" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
         <v>459</v>
       </c>
@@ -6104,7 +6122,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="15.95">
+    <row r="184" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="5" t="s">
         <v>461</v>
       </c>
@@ -6122,7 +6140,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="32.1">
+    <row r="185" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="6" t="s">
         <v>462</v>
       </c>
@@ -6140,7 +6158,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="15.95">
+    <row r="186" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="5" t="s">
         <v>464</v>
       </c>
@@ -6160,7 +6178,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="15.95">
+    <row r="187" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="13" t="s">
         <v>467</v>
       </c>
@@ -6178,7 +6196,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="15.95">
+    <row r="188" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="8" t="s">
         <v>468</v>
       </c>
@@ -6196,7 +6214,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="15.95">
+    <row r="189" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="8" t="s">
         <v>469</v>
       </c>
@@ -6214,7 +6232,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="15.95">
+    <row r="190" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="5" t="s">
         <v>470</v>
       </c>
@@ -6234,7 +6252,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="15.95">
+    <row r="191" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="8" t="s">
         <v>347</v>
       </c>
@@ -6252,7 +6270,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="36">
+    <row r="192" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A192" s="8" t="s">
         <v>472</v>
       </c>
@@ -6270,7 +6288,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="15.95">
+    <row r="193" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="5" t="s">
         <v>475</v>
       </c>
@@ -6288,7 +6306,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="15.95">
+    <row r="194" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="5" t="s">
         <v>477</v>
       </c>
@@ -6306,7 +6324,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="15.95">
+    <row r="195" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="5" t="s">
         <v>479</v>
       </c>
@@ -6324,7 +6342,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="36">
+    <row r="196" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A196" s="6" t="s">
         <v>480</v>
       </c>
@@ -6342,7 +6360,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="15.95">
+    <row r="197" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="8" t="s">
         <v>482</v>
       </c>
@@ -6360,7 +6378,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="198" spans="1:6" ht="15.95">
+    <row r="198" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="8" t="s">
         <v>483</v>
       </c>
@@ -6378,7 +6396,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="15.95">
+    <row r="199" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="5" t="s">
         <v>484</v>
       </c>
@@ -6398,7 +6416,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="32.1">
+    <row r="200" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="8" t="s">
         <v>487</v>
       </c>
@@ -6416,7 +6434,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="201" spans="1:6" ht="15.95">
+    <row r="201" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="5" t="s">
         <v>488</v>
       </c>
@@ -6432,7 +6450,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="15.95">
+    <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="8" t="s">
         <v>491</v>
       </c>
@@ -6450,7 +6468,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="15.95">
+    <row r="203" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="6" t="s">
         <v>492</v>
       </c>
@@ -6468,7 +6486,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="15.95">
+    <row r="204" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="5" t="s">
         <v>493</v>
       </c>
@@ -6484,7 +6502,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="120">
+    <row r="205" spans="1:6" ht="120" x14ac:dyDescent="0.2">
       <c r="A205" s="7" t="s">
         <v>495</v>
       </c>
@@ -6504,7 +6522,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="15.95">
+    <row r="206" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="5" t="s">
         <v>498</v>
       </c>
@@ -6522,7 +6540,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="15.95">
+    <row r="207" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="7" t="s">
         <v>500</v>
       </c>
@@ -6542,7 +6560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="15.95">
+    <row r="208" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="6" t="s">
         <v>503</v>
       </c>
@@ -6560,7 +6578,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="48">
+    <row r="209" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A209" s="6" t="s">
         <v>505</v>
       </c>
@@ -6580,7 +6598,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="15.95">
+    <row r="210" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" s="5" t="s">
         <v>509</v>
       </c>
@@ -6598,7 +6616,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="15.95">
+    <row r="211" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A211" s="6" t="s">
         <v>510</v>
       </c>
@@ -6616,7 +6634,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="15.95">
+    <row r="212" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A212" s="6" t="s">
         <v>511</v>
       </c>
@@ -6634,7 +6652,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="24">
+    <row r="213" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A213" s="8" t="s">
         <v>513</v>
       </c>
@@ -6652,7 +6670,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="15.95">
+    <row r="214" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="5" t="s">
         <v>515</v>
       </c>
@@ -6670,7 +6688,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="36">
+    <row r="215" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A215" s="5" t="s">
         <v>517</v>
       </c>
@@ -6688,7 +6706,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="15.95">
+    <row r="216" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="6" t="s">
         <v>520</v>
       </c>
@@ -6706,7 +6724,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="15.95">
+    <row r="217" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="6" t="s">
         <v>521</v>
       </c>
@@ -6724,7 +6742,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="15.95">
+    <row r="218" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="6" t="s">
         <v>522</v>
       </c>
@@ -6742,7 +6760,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="15.95">
+    <row r="219" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A219" s="8" t="s">
         <v>523</v>
       </c>
@@ -6761,7 +6779,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="15.95">
+    <row r="220" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="6" t="s">
         <v>526</v>
       </c>
@@ -6779,7 +6797,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="15.95">
+    <row r="221" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="6" t="s">
         <v>528</v>
       </c>
@@ -6797,7 +6815,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="15.95">
+    <row r="222" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="5" t="s">
         <v>529</v>
       </c>
@@ -6815,7 +6833,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="15.95">
+    <row r="223" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="5" t="s">
         <v>530</v>
       </c>
@@ -6835,7 +6853,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="15.95">
+    <row r="224" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="5" t="s">
         <v>533</v>
       </c>
@@ -6853,7 +6871,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="24">
+    <row r="225" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A225" s="8" t="s">
         <v>534</v>
       </c>
@@ -6871,7 +6889,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="226" spans="1:6" ht="15.95">
+    <row r="226" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A226" s="5" t="s">
         <v>535</v>
       </c>
@@ -6889,7 +6907,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="15.95">
+    <row r="227" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" s="6" t="s">
         <v>536</v>
       </c>
@@ -6907,7 +6925,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="228" spans="1:6" ht="15.95">
+    <row r="228" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="6" t="s">
         <v>537</v>
       </c>
@@ -6925,7 +6943,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="229" spans="1:6" ht="15.95">
+    <row r="229" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" s="6" t="s">
         <v>538</v>
       </c>
@@ -6943,7 +6961,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="230" spans="1:6" ht="15.95">
+    <row r="230" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A230" s="6" t="s">
         <v>539</v>
       </c>
@@ -6961,7 +6979,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="15.95">
+    <row r="231" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A231" s="6" t="s">
         <v>540</v>
       </c>
@@ -6979,7 +6997,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="15.95">
+    <row r="232" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A232" s="6" t="s">
         <v>541</v>
       </c>
@@ -6997,7 +7015,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="15.95">
+    <row r="233" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A233" s="6" t="s">
         <v>542</v>
       </c>
@@ -7015,7 +7033,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="15.95">
+    <row r="234" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A234" s="5" t="s">
         <v>543</v>
       </c>
@@ -7035,7 +7053,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="15.95">
+    <row r="235" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A235" s="5" t="s">
         <v>545</v>
       </c>
@@ -7055,7 +7073,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="236" spans="1:6" ht="15.95">
+    <row r="236" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A236" s="5" t="s">
         <v>547</v>
       </c>
@@ -7075,7 +7093,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="15.95">
+    <row r="237" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A237" s="6" t="s">
         <v>549</v>
       </c>
@@ -7093,7 +7111,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="15.95">
+    <row r="238" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A238" s="5" t="s">
         <v>550</v>
       </c>
@@ -7113,7 +7131,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="239" spans="1:6" ht="15.95">
+    <row r="239" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A239" s="5" t="s">
         <v>552</v>
       </c>
@@ -7133,7 +7151,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="240" spans="1:6" ht="15.95">
+    <row r="240" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A240" s="5" t="s">
         <v>554</v>
       </c>
@@ -7153,7 +7171,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="32.1">
+    <row r="241" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A241" s="16" t="s">
         <v>557</v>
       </c>
@@ -7169,7 +7187,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="242" spans="1:6" ht="36">
+    <row r="242" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A242" s="5" t="s">
         <v>560</v>
       </c>
@@ -7187,7 +7205,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="243" spans="1:6" ht="36">
+    <row r="243" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A243" s="5" t="s">
         <v>563</v>
       </c>
@@ -7205,7 +7223,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="244" spans="1:6" ht="36">
+    <row r="244" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A244" s="4" t="s">
         <v>566</v>
       </c>
@@ -7223,91 +7241,103 @@
         <v>250</v>
       </c>
     </row>
-    <row r="250" spans="1:6">
+    <row r="245" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A245" s="39" t="s">
+        <v>568</v>
+      </c>
+      <c r="B245" s="40"/>
+      <c r="C245" s="41" t="s">
+        <v>569</v>
+      </c>
+      <c r="D245" s="42"/>
+      <c r="E245" s="40"/>
+      <c r="F245" s="40"/>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" s="2"/>
       <c r="C250" s="2"/>
     </row>
-    <row r="251" spans="1:6">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" s="2"/>
       <c r="C251" s="2"/>
     </row>
-    <row r="256" spans="1:6">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256" s="2"/>
       <c r="C256" s="2"/>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="2"/>
       <c r="C257" s="2"/>
     </row>
-    <row r="258" spans="1:3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="2"/>
       <c r="C258" s="2"/>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="2"/>
       <c r="C259" s="2"/>
     </row>
-    <row r="260" spans="1:3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="2"/>
       <c r="C260" s="2"/>
     </row>
-    <row r="261" spans="1:3">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="2"/>
       <c r="C261" s="2"/>
     </row>
-    <row r="341" spans="1:3">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341" s="2"/>
       <c r="C341" s="2"/>
     </row>
-    <row r="342" spans="1:3">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342" s="2"/>
       <c r="C342" s="2"/>
     </row>
-    <row r="352" spans="1:3">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352" s="2"/>
       <c r="C352" s="2"/>
     </row>
-    <row r="354" spans="1:3">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354" s="2"/>
       <c r="C354" s="2"/>
     </row>
-    <row r="418" spans="1:3">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418" s="2"/>
       <c r="C418" s="2"/>
     </row>
-    <row r="419" spans="1:3">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419" s="2"/>
       <c r="C419" s="2"/>
     </row>
-    <row r="426" spans="1:3">
+    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A426" s="2"/>
       <c r="C426" s="2"/>
     </row>
-    <row r="427" spans="1:3">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A427" s="2"/>
       <c r="C427" s="2"/>
     </row>
-    <row r="435" spans="1:3">
+    <row r="435" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A435" s="2"/>
       <c r="C435" s="2"/>
     </row>
-    <row r="436" spans="1:3">
+    <row r="436" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A436" s="2"/>
       <c r="C436" s="2"/>
     </row>
-    <row r="459" spans="1:3">
+    <row r="459" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A459" s="2"/>
       <c r="C459" s="2"/>
     </row>
-    <row r="460" spans="1:3">
+    <row r="460" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A460" s="2"/>
       <c r="C460" s="2"/>
     </row>
-    <row r="491" spans="1:3">
+    <row r="491" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A491" s="2"/>
       <c r="C491" s="2"/>
     </row>
-    <row r="492" spans="1:3">
+    <row r="492" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A492" s="2"/>
       <c r="C492" s="2"/>
     </row>
@@ -7529,12 +7559,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -7543,14 +7567,44 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E603311A-CB77-4222-8BE5-7C219C89ED79}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E603311A-CB77-4222-8BE5-7C219C89ED79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e0a64e4-7fea-442c-b385-37491aef63de"/>
+    <ds:schemaRef ds:uri="2b3e05ff-c908-49af-94f9-52f298489e32"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94971B3D-2653-467D-B31F-1772BBCE73FC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{615F9342-5B50-4FC5-8179-20070E4D077E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{615F9342-5B50-4FC5-8179-20070E4D077E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94971B3D-2653-467D-B31F-1772BBCE73FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>